<commit_message>
additional changes after feedback
</commit_message>
<xml_diff>
--- a/teaching-cases/sprandel-inc/downloads/Workpapers.xlsx
+++ b/teaching-cases/sprandel-inc/downloads/Workpapers.xlsx
@@ -1192,6 +1192,18 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -1200,18 +1212,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -1955,7 +1955,7 @@
   <dimension ref="A1:G50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:F2"/>
+      <selection activeCell="H36" sqref="H36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="13.5" x14ac:dyDescent="0.2"/>
@@ -2535,7 +2535,7 @@
         <v>91</v>
       </c>
       <c r="E36" s="24">
-        <v>287483.13</v>
+        <v>278483.13</v>
       </c>
       <c r="F36" s="25" t="s">
         <v>24</v>
@@ -2750,36 +2750,36 @@
       <c r="A2" s="86" t="s">
         <v>114</v>
       </c>
-      <c r="B2" s="99"/>
-      <c r="C2" s="99"/>
-      <c r="D2" s="99"/>
-      <c r="E2" s="99"/>
-      <c r="F2" s="99"/>
-      <c r="G2" s="99"/>
+      <c r="B2" s="103"/>
+      <c r="C2" s="103"/>
+      <c r="D2" s="103"/>
+      <c r="E2" s="103"/>
+      <c r="F2" s="103"/>
+      <c r="G2" s="103"/>
       <c r="H2" s="2"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="86" t="s">
         <v>61</v>
       </c>
-      <c r="B3" s="99"/>
-      <c r="C3" s="99"/>
-      <c r="D3" s="99"/>
-      <c r="E3" s="99"/>
-      <c r="F3" s="99"/>
-      <c r="G3" s="99"/>
+      <c r="B3" s="103"/>
+      <c r="C3" s="103"/>
+      <c r="D3" s="103"/>
+      <c r="E3" s="103"/>
+      <c r="F3" s="103"/>
+      <c r="G3" s="103"/>
       <c r="H3" s="2"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="86" t="s">
         <v>67</v>
       </c>
-      <c r="B4" s="99"/>
-      <c r="C4" s="99"/>
-      <c r="D4" s="99"/>
-      <c r="E4" s="99"/>
-      <c r="F4" s="99"/>
-      <c r="G4" s="99"/>
+      <c r="B4" s="103"/>
+      <c r="C4" s="103"/>
+      <c r="D4" s="103"/>
+      <c r="E4" s="103"/>
+      <c r="F4" s="103"/>
+      <c r="G4" s="103"/>
       <c r="H4" s="2"/>
     </row>
     <row r="5" spans="1:14" ht="14.25" thickBot="1" x14ac:dyDescent="0.25"/>
@@ -2787,34 +2787,34 @@
       <c r="A6" s="83" t="s">
         <v>138</v>
       </c>
-      <c r="B6" s="97"/>
-      <c r="C6" s="97"/>
-      <c r="D6" s="97"/>
-      <c r="E6" s="97"/>
-      <c r="F6" s="97"/>
-      <c r="G6" s="98"/>
+      <c r="B6" s="101"/>
+      <c r="C6" s="101"/>
+      <c r="D6" s="101"/>
+      <c r="E6" s="101"/>
+      <c r="F6" s="101"/>
+      <c r="G6" s="102"/>
     </row>
     <row r="7" spans="1:14" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="92" t="s">
         <v>149</v>
       </c>
-      <c r="B7" s="97"/>
-      <c r="C7" s="97"/>
-      <c r="D7" s="97"/>
-      <c r="E7" s="97"/>
-      <c r="F7" s="97"/>
-      <c r="G7" s="98"/>
+      <c r="B7" s="101"/>
+      <c r="C7" s="101"/>
+      <c r="D7" s="101"/>
+      <c r="E7" s="101"/>
+      <c r="F7" s="101"/>
+      <c r="G7" s="102"/>
     </row>
     <row r="8" spans="1:14" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="92" t="s">
         <v>140</v>
       </c>
-      <c r="B8" s="97"/>
-      <c r="C8" s="97"/>
-      <c r="D8" s="97"/>
-      <c r="E8" s="97"/>
-      <c r="F8" s="97"/>
-      <c r="G8" s="98"/>
+      <c r="B8" s="101"/>
+      <c r="C8" s="101"/>
+      <c r="D8" s="101"/>
+      <c r="E8" s="101"/>
+      <c r="F8" s="101"/>
+      <c r="G8" s="102"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="52"/>
@@ -2940,14 +2940,14 @@
       <c r="A24" s="48" t="s">
         <v>63</v>
       </c>
-      <c r="B24" s="100" t="s">
+      <c r="B24" s="97" t="s">
         <v>108</v>
       </c>
-      <c r="C24" s="100"/>
-      <c r="D24" s="100"/>
-      <c r="E24" s="100"/>
-      <c r="F24" s="100"/>
-      <c r="G24" s="100"/>
+      <c r="C24" s="97"/>
+      <c r="D24" s="97"/>
+      <c r="E24" s="97"/>
+      <c r="F24" s="97"/>
+      <c r="G24" s="97"/>
     </row>
     <row r="25" spans="1:10" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A25" s="72" t="s">
@@ -2983,9 +2983,9 @@
       <c r="E27" s="87"/>
       <c r="F27" s="87"/>
       <c r="G27" s="87"/>
-      <c r="H27" s="101"/>
-      <c r="I27" s="102"/>
-      <c r="J27" s="102"/>
+      <c r="H27" s="98"/>
+      <c r="I27" s="99"/>
+      <c r="J27" s="99"/>
     </row>
     <row r="28" spans="1:10" ht="7.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="47"/>
@@ -3023,28 +3023,28 @@
       <c r="A31" s="48" t="s">
         <v>51</v>
       </c>
-      <c r="B31" s="103" t="s">
+      <c r="B31" s="100" t="s">
         <v>148</v>
       </c>
-      <c r="C31" s="103"/>
-      <c r="D31" s="103"/>
-      <c r="E31" s="103"/>
-      <c r="F31" s="103"/>
-      <c r="G31" s="103"/>
+      <c r="C31" s="100"/>
+      <c r="D31" s="100"/>
+      <c r="E31" s="100"/>
+      <c r="F31" s="100"/>
+      <c r="G31" s="100"/>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A22:G22"/>
-    <mergeCell ref="B24:G24"/>
-    <mergeCell ref="H27:J27"/>
-    <mergeCell ref="B27:G27"/>
-    <mergeCell ref="B31:G31"/>
     <mergeCell ref="A8:G8"/>
     <mergeCell ref="A6:G6"/>
     <mergeCell ref="A7:G7"/>
     <mergeCell ref="A4:G4"/>
     <mergeCell ref="A2:G2"/>
     <mergeCell ref="A3:G3"/>
+    <mergeCell ref="A22:G22"/>
+    <mergeCell ref="B24:G24"/>
+    <mergeCell ref="H27:J27"/>
+    <mergeCell ref="B27:G27"/>
+    <mergeCell ref="B31:G31"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3117,31 +3117,31 @@
       <c r="A6" s="83" t="s">
         <v>142</v>
       </c>
-      <c r="B6" s="97"/>
-      <c r="C6" s="97"/>
-      <c r="D6" s="97"/>
-      <c r="E6" s="97"/>
-      <c r="F6" s="98"/>
+      <c r="B6" s="101"/>
+      <c r="C6" s="101"/>
+      <c r="D6" s="101"/>
+      <c r="E6" s="101"/>
+      <c r="F6" s="102"/>
     </row>
     <row r="7" spans="1:7" ht="48.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="92" t="s">
         <v>150</v>
       </c>
-      <c r="B7" s="97"/>
-      <c r="C7" s="97"/>
-      <c r="D7" s="97"/>
-      <c r="E7" s="97"/>
-      <c r="F7" s="98"/>
+      <c r="B7" s="101"/>
+      <c r="C7" s="101"/>
+      <c r="D7" s="101"/>
+      <c r="E7" s="101"/>
+      <c r="F7" s="102"/>
     </row>
     <row r="8" spans="1:7" ht="37.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="92" t="s">
         <v>143</v>
       </c>
-      <c r="B8" s="97"/>
-      <c r="C8" s="97"/>
-      <c r="D8" s="97"/>
-      <c r="E8" s="97"/>
-      <c r="F8" s="98"/>
+      <c r="B8" s="101"/>
+      <c r="C8" s="101"/>
+      <c r="D8" s="101"/>
+      <c r="E8" s="101"/>
+      <c r="F8" s="102"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
@@ -3880,34 +3880,34 @@
       <c r="A6" s="83" t="s">
         <v>158</v>
       </c>
-      <c r="B6" s="97"/>
-      <c r="C6" s="97"/>
-      <c r="D6" s="97"/>
-      <c r="E6" s="97"/>
-      <c r="F6" s="97"/>
-      <c r="G6" s="98"/>
+      <c r="B6" s="101"/>
+      <c r="C6" s="101"/>
+      <c r="D6" s="101"/>
+      <c r="E6" s="101"/>
+      <c r="F6" s="101"/>
+      <c r="G6" s="102"/>
     </row>
     <row r="7" spans="1:7" ht="127.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="92" t="s">
         <v>153</v>
       </c>
-      <c r="B7" s="97"/>
-      <c r="C7" s="97"/>
-      <c r="D7" s="97"/>
-      <c r="E7" s="97"/>
-      <c r="F7" s="97"/>
-      <c r="G7" s="98"/>
+      <c r="B7" s="101"/>
+      <c r="C7" s="101"/>
+      <c r="D7" s="101"/>
+      <c r="E7" s="101"/>
+      <c r="F7" s="101"/>
+      <c r="G7" s="102"/>
     </row>
     <row r="8" spans="1:7" ht="43.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="92" t="s">
         <v>154</v>
       </c>
-      <c r="B8" s="97"/>
-      <c r="C8" s="97"/>
-      <c r="D8" s="97"/>
-      <c r="E8" s="97"/>
-      <c r="F8" s="97"/>
-      <c r="G8" s="98"/>
+      <c r="B8" s="101"/>
+      <c r="C8" s="101"/>
+      <c r="D8" s="101"/>
+      <c r="E8" s="101"/>
+      <c r="F8" s="101"/>
+      <c r="G8" s="102"/>
     </row>
     <row r="9" spans="1:7" ht="14.25" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="10" spans="1:7" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">

</xml_diff>